<commit_message>
Der corrections plan de tests
</commit_message>
<xml_diff>
--- a/plantest/P5_02_plantests.xlsx
+++ b/plantest/P5_02_plantests.xlsx
@@ -49,31 +49,16 @@
     <t>function init()</t>
   </si>
   <si>
-    <t>13 à 19</t>
-  </si>
-  <si>
     <t>function add(idProd)</t>
-  </si>
-  <si>
-    <t>21 à 30</t>
   </si>
   <si>
     <t>function remove(idProd)</t>
   </si>
   <si>
-    <t>32 à 34</t>
-  </si>
-  <si>
     <t>function clear()</t>
   </si>
   <si>
-    <t>parser le retour de la base de données et vérifier le contenu de chaque objet via console.log</t>
-  </si>
-  <si>
     <t>Le retour obtenu pourrait être erroné ou vide</t>
-  </si>
-  <si>
-    <t>Réception ou envoi à l'adresse url de la base de données, ainsi que de données et indication de leur type, si envoi</t>
   </si>
   <si>
     <t xml:space="preserve">request.onreadystatechange = function () {if (request.readyState === 4) {if(request.status === 200 || request.status === 201) </t>
@@ -85,22 +70,7 @@
     <t>Etapes de 0 à 4 de la création du client XMLHttpRequest à l'opération de récupération terminée ; et statut de l'objet XMLHttpRequest</t>
   </si>
   <si>
-    <t>9 à 22</t>
-  </si>
-  <si>
-    <t>3 à 33</t>
-  </si>
-  <si>
     <t>Utiliser page Sources ou Débogueur de l'outil développement du navigateur, faire un brekpoint sur readyState (ligne 12) et status (ligne 14) pour connaître le résultat dans Scope (Chrome)</t>
-  </si>
-  <si>
-    <t>Créer une key et retourner ses values en tableau JSON</t>
-  </si>
-  <si>
-    <t>Via Application de l'outil développement du navigateur voir si le LocalStorage contient au moins la key (ici panier) et des values si elles ont été ajoutées dans un tableau JSON [","]</t>
-  </si>
-  <si>
-    <t>La key pourrait ne pas être présente et ne pas retourner les values au format JSON</t>
   </si>
   <si>
     <t xml:space="preserve">Via Application de l'outil développement du navigateur voir si le LocalStorage le tableau JSON des values de la Key panier contient le nouveau id du produit </t>
@@ -128,6 +98,36 @@
   </si>
   <si>
     <t>Key panier pourrait subsisté ainsi que son contenu</t>
+  </si>
+  <si>
+    <t>Via Application de l'outil développement du navigateur voir si le LocalStorage contient au moins la key (ici basket) et des values si elles ont été ajoutées dans un tableau JSON [","]</t>
+  </si>
+  <si>
+    <t>Créer un key et retourner ses values en tableau JSON si on a ajouté une caméra via produit.js, sinon rien</t>
+  </si>
+  <si>
+    <t>Le key pourrait ne pas être présent et ne pas retourner les values au format JSON après un ajout via produit,js</t>
+  </si>
+  <si>
+    <t>10 à 22</t>
+  </si>
+  <si>
+    <t>4 à 34</t>
+  </si>
+  <si>
+    <t>Connaître la method, l'url, les données et le type de données</t>
+  </si>
+  <si>
+    <t>Utiliser console.log en indiquant le type de paramètre attendu suivi du paramètre</t>
+  </si>
+  <si>
+    <t>14 à 21</t>
+  </si>
+  <si>
+    <t>24 à 34</t>
+  </si>
+  <si>
+    <t>37 à 39</t>
   </si>
 </sst>
 </file>
@@ -465,9 +465,9 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -525,37 +525,37 @@
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="121.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -569,67 +569,67 @@
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="15" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrections sans prettier, inégalité stricte et cart au lieu de basket
</commit_message>
<xml_diff>
--- a/plantest/P5_02_plantests.xlsx
+++ b/plantest/P5_02_plantests.xlsx
@@ -70,43 +70,13 @@
     <t>Etapes de 0 à 4 de la création du client XMLHttpRequest à l'opération de récupération terminée ; et statut de l'objet XMLHttpRequest</t>
   </si>
   <si>
-    <t>Utiliser page Sources ou Débogueur de l'outil développement du navigateur, faire un brekpoint sur readyState (ligne 12) et status (ligne 14) pour connaître le résultat dans Scope (Chrome)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Via Application de l'outil développement du navigateur voir si le LocalStorage le tableau JSON des values de la Key panier contient le nouveau id du produit </t>
-  </si>
-  <si>
     <t>Le id du produit pourrait être null ou ne pas appraître dans le tableau Values ou le tableau Values ne pas être un tableau au format JSON dans LocalStorage</t>
-  </si>
-  <si>
-    <t>Ajouter le id du produit à mettre dans le panier en fin du tableau values de la key panier du LocalStorage</t>
-  </si>
-  <si>
-    <t>Filtrer les id de produit n'étant pas celui à supprimer du panier dans le tableau de la key panier dans le LocalStorage pour les réinjecter dans Values</t>
-  </si>
-  <si>
-    <t>Via Application de l'outil développement du navigateur voir si le LocalStorage le tableau JSON des values de la Key panier contient les id du produit sauf celui supprimé</t>
   </si>
   <si>
     <t>Le tableau Values pourrait être vide ou n'avoir pas changé, il pourrait aussi ne plus être en JSON</t>
   </si>
   <si>
-    <t>Suppression de la key panier et de son contenu dans le LocalStorage</t>
-  </si>
-  <si>
-    <t>Via Application de l'outil développement du navigateur voir si le LocalStorage ne contient ni key panier ni son contenu</t>
-  </si>
-  <si>
-    <t>Key panier pourrait subsisté ainsi que son contenu</t>
-  </si>
-  <si>
-    <t>Via Application de l'outil développement du navigateur voir si le LocalStorage contient au moins la key (ici basket) et des values si elles ont été ajoutées dans un tableau JSON [","]</t>
-  </si>
-  <si>
     <t>Créer un key et retourner ses values en tableau JSON si on a ajouté une caméra via produit.js, sinon rien</t>
-  </si>
-  <si>
-    <t>Le key pourrait ne pas être présent et ne pas retourner les values au format JSON après un ajout via produit,js</t>
   </si>
   <si>
     <t>10 à 22</t>
@@ -118,9 +88,6 @@
     <t>Connaître la method, l'url, les données et le type de données</t>
   </si>
   <si>
-    <t>Utiliser console.log en indiquant le type de paramètre attendu suivi du paramètre</t>
-  </si>
-  <si>
     <t>14 à 21</t>
   </si>
   <si>
@@ -128,6 +95,40 @@
   </si>
   <si>
     <t>37 à 39</t>
+  </si>
+  <si>
+    <t>Décommenter le console.log en ligne 25, résultat apparaîtra  dans l"outil Console du navigateur au chargement de la page index,html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Au chargement de la page  index.html et au click sur le bouton Commander en page panier.html
+Utiliser page Sources ou Débogueur de l'outil développement du navigateur, faire un brekpoint sur readyState (ligne 13) et un status (ligne 15), pour connaître le résultat dans Scope (Chrome) : les deux pages doivent indiquer dans le  prototype XMLHttpRequest 5 étapes allant de 0 à 4 pour la ligne 13,  puis  un status === 200 en page index.html et  un status === 201 en page panier.html pour la ligne 15</t>
+  </si>
+  <si>
+    <t>Le key pourrait ne pas être présent et/ou ne pas retourner les values en JSON</t>
+  </si>
+  <si>
+    <t>Après avoir cliqué sur Ajouter au panier en page produit.js, via Application de l'outil développement du navigateur voir si le LocalStorage contient au moins le key (ici cart) et au moins une value dans un tableau JSON [","]</t>
+  </si>
+  <si>
+    <t>Après avoir cliqué sur Ajouter au panier en page produit.js, via Application de l'outil développement du navigateur voir si le LocalStorage le tableau JSON des values de la Key panier contient le nouveau id du produit à la fin des values</t>
+  </si>
+  <si>
+    <t>Filtrer les id de produit n'étant pas celui à supprimer du panier dans le tableau de la key cart dans le LocalStorage pour les réinjecter dans Values</t>
+  </si>
+  <si>
+    <t>Après avoir cliqué sur picto poubelle en page panier.js, via Application de l'outil développement du navigateur voir si le LocalStorage le tableau JSON des values de la Key cart  ne contient plus le id du produit supprimé</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Après avoir cliqué sur Commander en page panier,html et avoir été redirigé vers la page commande,html, via Application de l'outil développement du navigateur voir si le LocalStorage ne contient ni key cart ni ses values</t>
+  </si>
+  <si>
+    <t>Suppression de la key cart et ses values dans le LocalStorage</t>
+  </si>
+  <si>
+    <t>Key cart pourrait subsisté ainsi que  ses values</t>
+  </si>
+  <si>
+    <t>Ajouter le id du produit en fin du tableau values de la key cart du LocalStorage</t>
   </si>
 </sst>
 </file>
@@ -467,7 +468,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -525,25 +526,25 @@
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="121.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="187.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>15</v>
@@ -552,13 +553,13 @@
         <v>17</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="91.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -569,67 +570,67 @@
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>